<commit_message>
Added in some graphing
</commit_message>
<xml_diff>
--- a/pandas_simple.xlsx
+++ b/pandas_simple.xlsx
@@ -1,25 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Source\ZebraFishDataAnalysis\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="112">
   <si>
     <t>group</t>
   </si>
@@ -33,209 +28,335 @@
     <t>sttime</t>
   </si>
   <si>
-    <t>23:28</t>
-  </si>
-  <si>
-    <t>23:38</t>
-  </si>
-  <si>
-    <t>23:48</t>
-  </si>
-  <si>
-    <t>23:58</t>
-  </si>
-  <si>
-    <t>00:08</t>
-  </si>
-  <si>
-    <t>00:18</t>
-  </si>
-  <si>
-    <t>00:28</t>
-  </si>
-  <si>
-    <t>00:38</t>
-  </si>
-  <si>
-    <t>00:48</t>
-  </si>
-  <si>
-    <t>00:58</t>
-  </si>
-  <si>
-    <t>01:08</t>
-  </si>
-  <si>
-    <t>01:18</t>
-  </si>
-  <si>
-    <t>01:28</t>
-  </si>
-  <si>
-    <t>01:38</t>
-  </si>
-  <si>
-    <t>01:48</t>
-  </si>
-  <si>
-    <t>01:58</t>
-  </si>
-  <si>
-    <t>02:08</t>
-  </si>
-  <si>
-    <t>02:18</t>
-  </si>
-  <si>
-    <t>02:28</t>
-  </si>
-  <si>
-    <t>02:38</t>
-  </si>
-  <si>
-    <t>02:48</t>
-  </si>
-  <si>
-    <t>02:58</t>
-  </si>
-  <si>
-    <t>03:08</t>
-  </si>
-  <si>
-    <t>03:18</t>
-  </si>
-  <si>
-    <t>03:28</t>
-  </si>
-  <si>
-    <t>03:38</t>
-  </si>
-  <si>
-    <t>03:48</t>
-  </si>
-  <si>
-    <t>03:58</t>
-  </si>
-  <si>
-    <t>04:08</t>
-  </si>
-  <si>
-    <t>04:18</t>
-  </si>
-  <si>
-    <t>04:28</t>
-  </si>
-  <si>
-    <t>04:38</t>
-  </si>
-  <si>
-    <t>04:48</t>
-  </si>
-  <si>
-    <t>04:58</t>
-  </si>
-  <si>
-    <t>05:08</t>
-  </si>
-  <si>
-    <t>05:18</t>
-  </si>
-  <si>
-    <t>05:28</t>
-  </si>
-  <si>
-    <t>05:38</t>
-  </si>
-  <si>
-    <t>05:48</t>
-  </si>
-  <si>
-    <t>05:58</t>
-  </si>
-  <si>
-    <t>06:08</t>
-  </si>
-  <si>
-    <t>06:18</t>
-  </si>
-  <si>
-    <t>06:28</t>
-  </si>
-  <si>
-    <t>06:38</t>
-  </si>
-  <si>
-    <t>06:48</t>
-  </si>
-  <si>
-    <t>06:58</t>
-  </si>
-  <si>
-    <t>07:08</t>
-  </si>
-  <si>
-    <t>07:18</t>
-  </si>
-  <si>
-    <t>07:28</t>
-  </si>
-  <si>
-    <t>07:38</t>
-  </si>
-  <si>
-    <t>07:48</t>
-  </si>
-  <si>
-    <t>07:58</t>
-  </si>
-  <si>
-    <t>08:08</t>
-  </si>
-  <si>
-    <t>08:18</t>
-  </si>
-  <si>
-    <t>08:28</t>
-  </si>
-  <si>
-    <t>08:38</t>
-  </si>
-  <si>
-    <t>08:48</t>
-  </si>
-  <si>
-    <t>08:58</t>
-  </si>
-  <si>
-    <t>09:08</t>
-  </si>
-  <si>
-    <t>09:18</t>
-  </si>
-  <si>
-    <t>09:28</t>
-  </si>
-  <si>
-    <t>09:38</t>
-  </si>
-  <si>
-    <t>09:48</t>
-  </si>
-  <si>
-    <t>09:58</t>
-  </si>
-  <si>
-    <t>10:08</t>
-  </si>
-  <si>
-    <t>10:18</t>
+    <t>23:28:03</t>
+  </si>
+  <si>
+    <t>23:28:04</t>
+  </si>
+  <si>
+    <t>23:38:04</t>
+  </si>
+  <si>
+    <t>23:48:03</t>
+  </si>
+  <si>
+    <t>23:48:04</t>
+  </si>
+  <si>
+    <t>23:58:03</t>
+  </si>
+  <si>
+    <t>23:58:04</t>
+  </si>
+  <si>
+    <t>00:08:03</t>
+  </si>
+  <si>
+    <t>00:08:04</t>
+  </si>
+  <si>
+    <t>00:18:03</t>
+  </si>
+  <si>
+    <t>00:18:04</t>
+  </si>
+  <si>
+    <t>00:28:03</t>
+  </si>
+  <si>
+    <t>00:28:04</t>
+  </si>
+  <si>
+    <t>00:38:03</t>
+  </si>
+  <si>
+    <t>00:38:04</t>
+  </si>
+  <si>
+    <t>00:48:03</t>
+  </si>
+  <si>
+    <t>00:48:04</t>
+  </si>
+  <si>
+    <t>00:58:03</t>
+  </si>
+  <si>
+    <t>00:58:04</t>
+  </si>
+  <si>
+    <t>01:08:03</t>
+  </si>
+  <si>
+    <t>01:08:04</t>
+  </si>
+  <si>
+    <t>01:18:03</t>
+  </si>
+  <si>
+    <t>01:18:04</t>
+  </si>
+  <si>
+    <t>01:28:03</t>
+  </si>
+  <si>
+    <t>01:28:04</t>
+  </si>
+  <si>
+    <t>01:38:03</t>
+  </si>
+  <si>
+    <t>01:38:04</t>
+  </si>
+  <si>
+    <t>01:48:03</t>
+  </si>
+  <si>
+    <t>01:48:04</t>
+  </si>
+  <si>
+    <t>01:58:03</t>
+  </si>
+  <si>
+    <t>01:58:04</t>
+  </si>
+  <si>
+    <t>02:08:03</t>
+  </si>
+  <si>
+    <t>02:08:04</t>
+  </si>
+  <si>
+    <t>02:18:03</t>
+  </si>
+  <si>
+    <t>02:18:04</t>
+  </si>
+  <si>
+    <t>02:28:03</t>
+  </si>
+  <si>
+    <t>02:28:04</t>
+  </si>
+  <si>
+    <t>02:38:03</t>
+  </si>
+  <si>
+    <t>02:38:04</t>
+  </si>
+  <si>
+    <t>02:48:03</t>
+  </si>
+  <si>
+    <t>02:48:04</t>
+  </si>
+  <si>
+    <t>02:58:04</t>
+  </si>
+  <si>
+    <t>03:08:04</t>
+  </si>
+  <si>
+    <t>03:18:04</t>
+  </si>
+  <si>
+    <t>03:28:04</t>
+  </si>
+  <si>
+    <t>03:38:04</t>
+  </si>
+  <si>
+    <t>03:48:04</t>
+  </si>
+  <si>
+    <t>03:58:04</t>
+  </si>
+  <si>
+    <t>04:08:04</t>
+  </si>
+  <si>
+    <t>04:18:04</t>
+  </si>
+  <si>
+    <t>04:28:03</t>
+  </si>
+  <si>
+    <t>04:28:04</t>
+  </si>
+  <si>
+    <t>04:38:03</t>
+  </si>
+  <si>
+    <t>04:38:04</t>
+  </si>
+  <si>
+    <t>04:48:03</t>
+  </si>
+  <si>
+    <t>04:48:04</t>
+  </si>
+  <si>
+    <t>04:58:03</t>
+  </si>
+  <si>
+    <t>04:58:04</t>
+  </si>
+  <si>
+    <t>05:08:04</t>
+  </si>
+  <si>
+    <t>05:18:03</t>
+  </si>
+  <si>
+    <t>05:18:04</t>
+  </si>
+  <si>
+    <t>05:28:04</t>
+  </si>
+  <si>
+    <t>05:38:04</t>
+  </si>
+  <si>
+    <t>05:48:03</t>
+  </si>
+  <si>
+    <t>05:48:04</t>
+  </si>
+  <si>
+    <t>05:58:04</t>
+  </si>
+  <si>
+    <t>06:08:03</t>
+  </si>
+  <si>
+    <t>06:08:04</t>
+  </si>
+  <si>
+    <t>06:18:03</t>
+  </si>
+  <si>
+    <t>06:18:04</t>
+  </si>
+  <si>
+    <t>06:28:03</t>
+  </si>
+  <si>
+    <t>06:28:04</t>
+  </si>
+  <si>
+    <t>06:38:03</t>
+  </si>
+  <si>
+    <t>06:38:04</t>
+  </si>
+  <si>
+    <t>06:48:03</t>
+  </si>
+  <si>
+    <t>06:48:04</t>
+  </si>
+  <si>
+    <t>06:58:03</t>
+  </si>
+  <si>
+    <t>06:58:04</t>
+  </si>
+  <si>
+    <t>07:08:03</t>
+  </si>
+  <si>
+    <t>07:08:04</t>
+  </si>
+  <si>
+    <t>07:18:03</t>
+  </si>
+  <si>
+    <t>07:18:06</t>
+  </si>
+  <si>
+    <t>07:28:03</t>
+  </si>
+  <si>
+    <t>07:28:04</t>
+  </si>
+  <si>
+    <t>07:38:04</t>
+  </si>
+  <si>
+    <t>07:48:03</t>
+  </si>
+  <si>
+    <t>07:48:04</t>
+  </si>
+  <si>
+    <t>07:58:04</t>
+  </si>
+  <si>
+    <t>08:08:04</t>
+  </si>
+  <si>
+    <t>08:18:04</t>
+  </si>
+  <si>
+    <t>08:28:03</t>
+  </si>
+  <si>
+    <t>08:28:04</t>
+  </si>
+  <si>
+    <t>08:38:03</t>
+  </si>
+  <si>
+    <t>08:38:04</t>
+  </si>
+  <si>
+    <t>08:48:03</t>
+  </si>
+  <si>
+    <t>08:48:04</t>
+  </si>
+  <si>
+    <t>08:58:04</t>
+  </si>
+  <si>
+    <t>09:08:04</t>
+  </si>
+  <si>
+    <t>09:18:04</t>
+  </si>
+  <si>
+    <t>09:28:04</t>
+  </si>
+  <si>
+    <t>09:38:04</t>
+  </si>
+  <si>
+    <t>09:48:03</t>
+  </si>
+  <si>
+    <t>09:48:04</t>
+  </si>
+  <si>
+    <t>09:58:04</t>
+  </si>
+  <si>
+    <t>10:08:03</t>
+  </si>
+  <si>
+    <t>10:08:04</t>
+  </si>
+  <si>
+    <t>10:18:03</t>
+  </si>
+  <si>
+    <t>10:18:04</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -298,14 +419,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -352,7 +465,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -384,10 +497,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -419,7 +531,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -595,16 +706,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E199"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -618,7 +727,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -626,16 +735,16 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>134.45625000000001</v>
+        <v>134.45625</v>
       </c>
       <c r="D2">
-        <v>33.721874999999997</v>
+        <v>33.721875</v>
       </c>
       <c r="E2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -646,13 +755,13 @@
         <v>182.1125000000001</v>
       </c>
       <c r="D3">
-        <v>39.075000000000003</v>
+        <v>39.075</v>
       </c>
       <c r="E3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -660,16 +769,16 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <v>258.37812500000001</v>
+        <v>258.378125</v>
       </c>
       <c r="D4">
-        <v>50.687499999999993</v>
+        <v>50.68749999999999</v>
       </c>
       <c r="E4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -677,16 +786,16 @@
         <v>1</v>
       </c>
       <c r="C5">
-        <v>80.790624999999977</v>
+        <v>80.79062499999998</v>
       </c>
       <c r="D5">
-        <v>22.737500000000001</v>
+        <v>22.7375</v>
       </c>
       <c r="E5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -694,16 +803,16 @@
         <v>2</v>
       </c>
       <c r="C6">
-        <v>68.893749999999997</v>
+        <v>68.89375</v>
       </c>
       <c r="D6">
         <v>18.3125</v>
       </c>
       <c r="E6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -717,10 +826,10 @@
         <v>31.40625</v>
       </c>
       <c r="E7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -731,13 +840,13 @@
         <v>122.09375</v>
       </c>
       <c r="D8">
-        <v>30.465624999999999</v>
+        <v>30.465625</v>
       </c>
       <c r="E8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -751,10 +860,10 @@
         <v>25.921875</v>
       </c>
       <c r="E9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -765,13 +874,13 @@
         <v>159.90625</v>
       </c>
       <c r="D10">
-        <v>36.421875000000007</v>
+        <v>36.42187500000001</v>
       </c>
       <c r="E10" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -779,16 +888,16 @@
         <v>1</v>
       </c>
       <c r="C11">
-        <v>100.13437500000001</v>
+        <v>100.134375</v>
       </c>
       <c r="D11">
-        <v>25.737500000000001</v>
+        <v>25.7375</v>
       </c>
       <c r="E11" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -796,16 +905,16 @@
         <v>2</v>
       </c>
       <c r="C12">
-        <v>114.06874999999999</v>
+        <v>114.06875</v>
       </c>
       <c r="D12">
-        <v>27.278124999999999</v>
+        <v>27.278125</v>
       </c>
       <c r="E12" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -813,16 +922,16 @@
         <v>3</v>
       </c>
       <c r="C13">
-        <v>176.30937499999999</v>
+        <v>176.309375</v>
       </c>
       <c r="D13">
-        <v>38.478124999999999</v>
+        <v>38.478125</v>
       </c>
       <c r="E13" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -830,16 +939,16 @@
         <v>1</v>
       </c>
       <c r="C14">
-        <v>86.590625000000017</v>
+        <v>86.59062500000002</v>
       </c>
       <c r="D14">
-        <v>23.303124999999991</v>
+        <v>23.30312499999999</v>
       </c>
       <c r="E14" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -847,16 +956,16 @@
         <v>2</v>
       </c>
       <c r="C15">
-        <v>88.709375000000023</v>
+        <v>88.70937500000002</v>
       </c>
       <c r="D15">
-        <v>21.746874999999999</v>
+        <v>21.746875</v>
       </c>
       <c r="E15" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -864,16 +973,16 @@
         <v>3</v>
       </c>
       <c r="C16">
-        <v>222.21562499999999</v>
+        <v>222.215625</v>
       </c>
       <c r="D16">
-        <v>47.021875000000001</v>
+        <v>47.021875</v>
       </c>
       <c r="E16" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -881,16 +990,16 @@
         <v>1</v>
       </c>
       <c r="C17">
-        <v>162.90624999999989</v>
+        <v>162.9062499999999</v>
       </c>
       <c r="D17">
-        <v>36.434375000000003</v>
+        <v>36.434375</v>
       </c>
       <c r="E17" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -901,13 +1010,13 @@
         <v>106.2</v>
       </c>
       <c r="D18">
-        <v>26.690625000000001</v>
+        <v>26.690625</v>
       </c>
       <c r="E18" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -915,16 +1024,16 @@
         <v>3</v>
       </c>
       <c r="C19">
-        <v>200.52812499999999</v>
+        <v>200.528125</v>
       </c>
       <c r="D19">
-        <v>45.903124999999989</v>
+        <v>45.90312499999999</v>
       </c>
       <c r="E19" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -932,16 +1041,16 @@
         <v>1</v>
       </c>
       <c r="C20">
-        <v>141.46562499999999</v>
+        <v>141.465625</v>
       </c>
       <c r="D20">
-        <v>31.534375000000001</v>
+        <v>31.534375</v>
       </c>
       <c r="E20" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -949,16 +1058,16 @@
         <v>2</v>
       </c>
       <c r="C21">
-        <v>120.33750000000001</v>
+        <v>120.3375</v>
       </c>
       <c r="D21">
-        <v>28.521875000000001</v>
+        <v>28.521875</v>
       </c>
       <c r="E21" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -966,16 +1075,16 @@
         <v>3</v>
       </c>
       <c r="C22">
-        <v>205.52812499999999</v>
+        <v>205.528125</v>
       </c>
       <c r="D22">
-        <v>42.862499999999997</v>
+        <v>42.8625</v>
       </c>
       <c r="E22" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -983,16 +1092,16 @@
         <v>1</v>
       </c>
       <c r="C23">
-        <v>98.165625000000006</v>
+        <v>98.16562500000001</v>
       </c>
       <c r="D23">
-        <v>27.115625000000001</v>
+        <v>27.115625</v>
       </c>
       <c r="E23" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -1000,16 +1109,16 @@
         <v>2</v>
       </c>
       <c r="C24">
-        <v>102.38437500000001</v>
+        <v>102.384375</v>
       </c>
       <c r="D24">
-        <v>25.871874999999999</v>
+        <v>25.871875</v>
       </c>
       <c r="E24" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -1020,13 +1129,13 @@
         <v>201.90625</v>
       </c>
       <c r="D25">
-        <v>41.725000000000001</v>
+        <v>41.725</v>
       </c>
       <c r="E25" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -1034,16 +1143,16 @@
         <v>1</v>
       </c>
       <c r="C26">
-        <v>160.64687499999999</v>
+        <v>160.646875</v>
       </c>
       <c r="D26">
-        <v>38.115625000000001</v>
+        <v>38.115625</v>
       </c>
       <c r="E26" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -1054,13 +1163,13 @@
         <v>112.29375</v>
       </c>
       <c r="D27">
-        <v>28.425000000000001</v>
+        <v>28.425</v>
       </c>
       <c r="E27" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -1068,16 +1177,16 @@
         <v>3</v>
       </c>
       <c r="C28">
-        <v>199.02812499999999</v>
+        <v>199.028125</v>
       </c>
       <c r="D28">
-        <v>43.659374999999997</v>
+        <v>43.659375</v>
       </c>
       <c r="E28" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -1085,16 +1194,16 @@
         <v>1</v>
       </c>
       <c r="C29">
-        <v>100.75624999999999</v>
+        <v>100.75625</v>
       </c>
       <c r="D29">
-        <v>28.528124999999999</v>
+        <v>28.528125</v>
       </c>
       <c r="E29" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -1105,13 +1214,13 @@
         <v>107.90625</v>
       </c>
       <c r="D30">
-        <v>25.290624999999999</v>
+        <v>25.290625</v>
       </c>
       <c r="E30" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -1119,16 +1228,16 @@
         <v>3</v>
       </c>
       <c r="C31">
-        <v>168.33125000000001</v>
+        <v>168.33125</v>
       </c>
       <c r="D31">
-        <v>39.568750000000001</v>
+        <v>39.56875</v>
       </c>
       <c r="E31" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -1139,13 +1248,13 @@
         <v>100.98125</v>
       </c>
       <c r="D32">
-        <v>27.996874999999999</v>
+        <v>27.996875</v>
       </c>
       <c r="E32" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -1153,16 +1262,16 @@
         <v>2</v>
       </c>
       <c r="C33">
-        <v>117.77500000000001</v>
+        <v>117.775</v>
       </c>
       <c r="D33">
-        <v>29.006250000000001</v>
+        <v>29.00625</v>
       </c>
       <c r="E33" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -1170,16 +1279,16 @@
         <v>3</v>
       </c>
       <c r="C34">
-        <v>172.81874999999999</v>
+        <v>172.81875</v>
       </c>
       <c r="D34">
-        <v>41.528125000000003</v>
+        <v>41.528125</v>
       </c>
       <c r="E34" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -1187,16 +1296,16 @@
         <v>1</v>
       </c>
       <c r="C35">
-        <v>84.565625000000011</v>
+        <v>84.56562500000001</v>
       </c>
       <c r="D35">
-        <v>26.768750000000001</v>
+        <v>26.76875</v>
       </c>
       <c r="E35" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -1204,16 +1313,16 @@
         <v>2</v>
       </c>
       <c r="C36">
-        <v>188.37187499999999</v>
+        <v>188.371875</v>
       </c>
       <c r="D36">
         <v>30.21875</v>
       </c>
       <c r="E36" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -1221,16 +1330,16 @@
         <v>3</v>
       </c>
       <c r="C37">
-        <v>186.37187499999999</v>
+        <v>186.371875</v>
       </c>
       <c r="D37">
-        <v>42.059375000000003</v>
+        <v>42.059375</v>
       </c>
       <c r="E37" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -1238,16 +1347,16 @@
         <v>1</v>
       </c>
       <c r="C38">
-        <v>142.54374999999999</v>
+        <v>142.54375</v>
       </c>
       <c r="D38">
-        <v>29.612500000000001</v>
+        <v>29.6125</v>
       </c>
       <c r="E38" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -1255,16 +1364,16 @@
         <v>2</v>
       </c>
       <c r="C39">
-        <v>181.32187500000001</v>
+        <v>181.321875</v>
       </c>
       <c r="D39">
-        <v>33.084374999999987</v>
+        <v>33.08437499999999</v>
       </c>
       <c r="E39" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -1272,16 +1381,16 @@
         <v>3</v>
       </c>
       <c r="C40">
-        <v>203.58437499999999</v>
+        <v>203.584375</v>
       </c>
       <c r="D40">
-        <v>42.990625000000001</v>
+        <v>42.990625</v>
       </c>
       <c r="E40" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -1289,16 +1398,16 @@
         <v>1</v>
       </c>
       <c r="C41">
-        <v>201.97187500000001</v>
+        <v>201.971875</v>
       </c>
       <c r="D41">
-        <v>43.256249999999987</v>
+        <v>43.25624999999999</v>
       </c>
       <c r="E41" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -1306,16 +1415,16 @@
         <v>2</v>
       </c>
       <c r="C42">
-        <v>135.69374999999999</v>
+        <v>135.69375</v>
       </c>
       <c r="D42">
-        <v>30.428125000000001</v>
+        <v>30.428125</v>
       </c>
       <c r="E42" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -1323,16 +1432,16 @@
         <v>3</v>
       </c>
       <c r="C43">
-        <v>231.15937500000001</v>
+        <v>231.159375</v>
       </c>
       <c r="D43">
         <v>47.92499999999999</v>
       </c>
       <c r="E43" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -1343,13 +1452,13 @@
         <v>164.40625</v>
       </c>
       <c r="D44">
-        <v>38.996875000000003</v>
+        <v>38.996875</v>
       </c>
       <c r="E44" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -1360,13 +1469,13 @@
         <v>107.3875</v>
       </c>
       <c r="D45">
-        <v>27.196874999999999</v>
+        <v>27.196875</v>
       </c>
       <c r="E45" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -1374,16 +1483,16 @@
         <v>3</v>
       </c>
       <c r="C46">
-        <v>252.75312500000001</v>
+        <v>252.753125</v>
       </c>
       <c r="D46">
-        <v>50.334375000000001</v>
+        <v>50.334375</v>
       </c>
       <c r="E46" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -1394,13 +1503,13 @@
         <v>311.5968749999999</v>
       </c>
       <c r="D47">
-        <v>43.990624999999987</v>
+        <v>43.99062499999999</v>
       </c>
       <c r="E47" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -1408,16 +1517,16 @@
         <v>2</v>
       </c>
       <c r="C48">
-        <v>153.81874999999999</v>
+        <v>153.81875</v>
       </c>
       <c r="D48">
         <v>30.15625</v>
       </c>
       <c r="E48" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -1425,16 +1534,16 @@
         <v>3</v>
       </c>
       <c r="C49">
-        <v>366.67187499999989</v>
+        <v>366.6718749999999</v>
       </c>
       <c r="D49">
-        <v>56.603125000000013</v>
+        <v>56.60312500000001</v>
       </c>
       <c r="E49" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -1442,16 +1551,16 @@
         <v>1</v>
       </c>
       <c r="C50">
-        <v>311.96249999999992</v>
+        <v>311.9624999999999</v>
       </c>
       <c r="D50">
-        <v>38.812500000000007</v>
+        <v>38.81250000000001</v>
       </c>
       <c r="E50" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -1459,16 +1568,16 @@
         <v>2</v>
       </c>
       <c r="C51">
-        <v>142.30937499999999</v>
+        <v>142.309375</v>
       </c>
       <c r="D51">
         <v>29.99687500000001</v>
       </c>
       <c r="E51" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -1476,16 +1585,16 @@
         <v>3</v>
       </c>
       <c r="C52">
-        <v>427.93124999999998</v>
+        <v>427.93125</v>
       </c>
       <c r="D52">
-        <v>57.671875000000007</v>
+        <v>57.67187500000001</v>
       </c>
       <c r="E52" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -1496,13 +1605,13 @@
         <v>367.3562500000001</v>
       </c>
       <c r="D53">
-        <v>42.643750000000011</v>
+        <v>42.64375000000001</v>
       </c>
       <c r="E53" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -1513,13 +1622,13 @@
         <v>97.61562499999998</v>
       </c>
       <c r="D54">
-        <v>26.725000000000001</v>
+        <v>26.725</v>
       </c>
       <c r="E54" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -1527,16 +1636,16 @@
         <v>3</v>
       </c>
       <c r="C55">
-        <v>339.26249999999999</v>
+        <v>339.2625</v>
       </c>
       <c r="D55">
-        <v>55.881250000000023</v>
+        <v>55.88125000000002</v>
       </c>
       <c r="E55" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -1550,10 +1659,10 @@
         <v>38.578125</v>
       </c>
       <c r="E56" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -1564,13 +1673,13 @@
         <v>112.171875</v>
       </c>
       <c r="D57">
-        <v>25.615625000000001</v>
+        <v>25.615625</v>
       </c>
       <c r="E57" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -1578,16 +1687,16 @@
         <v>3</v>
       </c>
       <c r="C58">
-        <v>486.80312500000002</v>
+        <v>486.803125</v>
       </c>
       <c r="D58">
         <v>69.421875</v>
       </c>
       <c r="E58" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -1595,16 +1704,16 @@
         <v>1</v>
       </c>
       <c r="C59">
-        <v>312.75625000000008</v>
+        <v>312.7562500000001</v>
       </c>
       <c r="D59">
-        <v>47.346874999999997</v>
+        <v>47.346875</v>
       </c>
       <c r="E59" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -1615,13 +1724,13 @@
         <v>179.55</v>
       </c>
       <c r="D60">
-        <v>36.431249999999991</v>
+        <v>36.43124999999999</v>
       </c>
       <c r="E60" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -1629,16 +1738,16 @@
         <v>3</v>
       </c>
       <c r="C61">
-        <v>410.81562500000001</v>
+        <v>410.815625</v>
       </c>
       <c r="D61">
-        <v>66.440624999999983</v>
+        <v>66.44062499999998</v>
       </c>
       <c r="E61" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
       <c r="A62" s="1">
         <v>60</v>
       </c>
@@ -1646,16 +1755,16 @@
         <v>1</v>
       </c>
       <c r="C62">
-        <v>232.45625000000001</v>
+        <v>232.45625</v>
       </c>
       <c r="D62">
-        <v>49.053125000000023</v>
+        <v>49.05312500000002</v>
       </c>
       <c r="E62" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
       <c r="A63" s="1">
         <v>61</v>
       </c>
@@ -1663,16 +1772,16 @@
         <v>2</v>
       </c>
       <c r="C63">
-        <v>147.66562500000001</v>
+        <v>147.665625</v>
       </c>
       <c r="D63">
-        <v>31.946874999999999</v>
+        <v>31.946875</v>
       </c>
       <c r="E63" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
       <c r="A64" s="1">
         <v>62</v>
       </c>
@@ -1680,16 +1789,16 @@
         <v>3</v>
       </c>
       <c r="C64">
-        <v>565.09062500000005</v>
+        <v>565.090625</v>
       </c>
       <c r="D64">
-        <v>66.165625000000006</v>
+        <v>66.16562500000001</v>
       </c>
       <c r="E64" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
       <c r="A65" s="1">
         <v>63</v>
       </c>
@@ -1700,13 +1809,13 @@
         <v>303.578125</v>
       </c>
       <c r="D65">
-        <v>56.984374999999993</v>
+        <v>56.98437499999999</v>
       </c>
       <c r="E65" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
       <c r="A66" s="1">
         <v>64</v>
       </c>
@@ -1717,13 +1826,13 @@
         <v>153.15</v>
       </c>
       <c r="D66">
-        <v>29.481249999999999</v>
+        <v>29.48125</v>
       </c>
       <c r="E66" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
       <c r="A67" s="1">
         <v>65</v>
       </c>
@@ -1731,16 +1840,16 @@
         <v>3</v>
       </c>
       <c r="C67">
-        <v>527.94687499999998</v>
+        <v>527.946875</v>
       </c>
       <c r="D67">
-        <v>63.149999999999991</v>
+        <v>63.14999999999999</v>
       </c>
       <c r="E67" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5">
       <c r="A68" s="1">
         <v>66</v>
       </c>
@@ -1748,16 +1857,16 @@
         <v>1</v>
       </c>
       <c r="C68">
-        <v>271.39375000000001</v>
+        <v>271.39375</v>
       </c>
       <c r="D68">
-        <v>49.703124999999993</v>
+        <v>49.70312499999999</v>
       </c>
       <c r="E68" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5">
       <c r="A69" s="1">
         <v>67</v>
       </c>
@@ -1768,13 +1877,13 @@
         <v>148.71875</v>
       </c>
       <c r="D69">
-        <v>29.943749999999991</v>
+        <v>29.94374999999999</v>
       </c>
       <c r="E69" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5">
       <c r="A70" s="1">
         <v>68</v>
       </c>
@@ -1782,16 +1891,16 @@
         <v>3</v>
       </c>
       <c r="C70">
-        <v>495.89999999999992</v>
+        <v>495.8999999999999</v>
       </c>
       <c r="D70">
-        <v>68.874999999999986</v>
+        <v>68.87499999999999</v>
       </c>
       <c r="E70" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5">
       <c r="A71" s="1">
         <v>69</v>
       </c>
@@ -1799,16 +1908,16 @@
         <v>1</v>
       </c>
       <c r="C71">
-        <v>408.33437500000008</v>
+        <v>408.3343750000001</v>
       </c>
       <c r="D71">
-        <v>53.043750000000017</v>
+        <v>53.04375000000002</v>
       </c>
       <c r="E71" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5">
       <c r="A72" s="1">
         <v>70</v>
       </c>
@@ -1816,16 +1925,16 @@
         <v>2</v>
       </c>
       <c r="C72">
-        <v>155.64687499999999</v>
+        <v>155.646875</v>
       </c>
       <c r="D72">
-        <v>32.896875000000001</v>
+        <v>32.896875</v>
       </c>
       <c r="E72" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5">
       <c r="A73" s="1">
         <v>71</v>
       </c>
@@ -1833,16 +1942,16 @@
         <v>3</v>
       </c>
       <c r="C73">
-        <v>423.88125000000002</v>
+        <v>423.88125</v>
       </c>
       <c r="D73">
-        <v>68.206249999999997</v>
+        <v>68.20625</v>
       </c>
       <c r="E73" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5">
       <c r="A74" s="1">
         <v>72</v>
       </c>
@@ -1850,16 +1959,16 @@
         <v>1</v>
       </c>
       <c r="C74">
-        <v>528.77812499999993</v>
+        <v>528.7781249999999</v>
       </c>
       <c r="D74">
-        <v>60.262500000000003</v>
+        <v>60.2625</v>
       </c>
       <c r="E74" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5">
       <c r="A75" s="1">
         <v>73</v>
       </c>
@@ -1867,16 +1976,16 @@
         <v>2</v>
       </c>
       <c r="C75">
-        <v>157.01249999999999</v>
+        <v>157.0125</v>
       </c>
       <c r="D75">
-        <v>32.809375000000003</v>
+        <v>32.809375</v>
       </c>
       <c r="E75" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5">
       <c r="A76" s="1">
         <v>74</v>
       </c>
@@ -1884,16 +1993,16 @@
         <v>3</v>
       </c>
       <c r="C76">
-        <v>491.08437500000002</v>
+        <v>491.084375</v>
       </c>
       <c r="D76">
-        <v>68.237500000000011</v>
+        <v>68.23750000000001</v>
       </c>
       <c r="E76" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5">
       <c r="A77" s="1">
         <v>75</v>
       </c>
@@ -1901,16 +2010,16 @@
         <v>1</v>
       </c>
       <c r="C77">
-        <v>516.03125000000011</v>
+        <v>516.0312500000001</v>
       </c>
       <c r="D77">
         <v>61.55</v>
       </c>
       <c r="E77" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5">
       <c r="A78" s="1">
         <v>76</v>
       </c>
@@ -1918,16 +2027,16 @@
         <v>2</v>
       </c>
       <c r="C78">
-        <v>182.19374999999999</v>
+        <v>182.19375</v>
       </c>
       <c r="D78">
-        <v>37.778125000000003</v>
+        <v>37.778125</v>
       </c>
       <c r="E78" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5">
       <c r="A79" s="1">
         <v>77</v>
       </c>
@@ -1935,16 +2044,16 @@
         <v>3</v>
       </c>
       <c r="C79">
-        <v>521.36562500000002</v>
+        <v>521.365625</v>
       </c>
       <c r="D79">
         <v>72.90000000000002</v>
       </c>
       <c r="E79" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5">
       <c r="A80" s="1">
         <v>78</v>
       </c>
@@ -1952,16 +2061,16 @@
         <v>1</v>
       </c>
       <c r="C80">
-        <v>352.91874999999999</v>
+        <v>352.91875</v>
       </c>
       <c r="D80">
-        <v>53.743750000000013</v>
+        <v>53.74375000000001</v>
       </c>
       <c r="E80" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5">
       <c r="A81" s="1">
         <v>79</v>
       </c>
@@ -1969,16 +2078,16 @@
         <v>2</v>
       </c>
       <c r="C81">
-        <v>85.715625000000003</v>
+        <v>85.715625</v>
       </c>
       <c r="D81">
         <v>25.26874999999999</v>
       </c>
       <c r="E81" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5">
       <c r="A82" s="1">
         <v>80</v>
       </c>
@@ -1986,16 +2095,16 @@
         <v>3</v>
       </c>
       <c r="C82">
-        <v>496.70312500000011</v>
+        <v>496.7031250000001</v>
       </c>
       <c r="D82">
-        <v>67.290625000000006</v>
+        <v>67.29062500000001</v>
       </c>
       <c r="E82" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5">
       <c r="A83" s="1">
         <v>81</v>
       </c>
@@ -2003,16 +2112,16 @@
         <v>1</v>
       </c>
       <c r="C83">
-        <v>270.42187500000011</v>
+        <v>270.4218750000001</v>
       </c>
       <c r="D83">
-        <v>44.946874999999999</v>
+        <v>44.946875</v>
       </c>
       <c r="E83" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5">
       <c r="A84" s="1">
         <v>82</v>
       </c>
@@ -2020,16 +2129,16 @@
         <v>2</v>
       </c>
       <c r="C84">
-        <v>117.30625000000001</v>
+        <v>117.30625</v>
       </c>
       <c r="D84">
-        <v>27.646875000000001</v>
+        <v>27.646875</v>
       </c>
       <c r="E84" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5">
       <c r="A85" s="1">
         <v>83</v>
       </c>
@@ -2037,16 +2146,16 @@
         <v>3</v>
       </c>
       <c r="C85">
-        <v>706.90624999999989</v>
+        <v>706.9062499999999</v>
       </c>
       <c r="D85">
-        <v>81.346875000000026</v>
+        <v>81.34687500000003</v>
       </c>
       <c r="E85" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5">
       <c r="A86" s="1">
         <v>84</v>
       </c>
@@ -2054,16 +2163,16 @@
         <v>1</v>
       </c>
       <c r="C86">
-        <v>534.83437499999991</v>
+        <v>534.8343749999999</v>
       </c>
       <c r="D86">
         <v>49.58124999999999</v>
       </c>
       <c r="E86" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5">
       <c r="A87" s="1">
         <v>85</v>
       </c>
@@ -2077,10 +2186,10 @@
         <v>28.71875</v>
       </c>
       <c r="E87" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5">
       <c r="A88" s="1">
         <v>86</v>
       </c>
@@ -2091,13 +2200,13 @@
         <v>595.4375</v>
       </c>
       <c r="D88">
-        <v>80.731250000000017</v>
+        <v>80.73125000000002</v>
       </c>
       <c r="E88" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5">
       <c r="A89" s="1">
         <v>87</v>
       </c>
@@ -2105,16 +2214,16 @@
         <v>1</v>
       </c>
       <c r="C89">
-        <v>613.49374999999998</v>
+        <v>613.49375</v>
       </c>
       <c r="D89">
-        <v>59.415624999999991</v>
+        <v>59.41562499999999</v>
       </c>
       <c r="E89" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5">
       <c r="A90" s="1">
         <v>88</v>
       </c>
@@ -2122,16 +2231,16 @@
         <v>2</v>
       </c>
       <c r="C90">
-        <v>157.39687499999999</v>
+        <v>157.396875</v>
       </c>
       <c r="D90">
         <v>32.46875</v>
       </c>
       <c r="E90" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5">
       <c r="A91" s="1">
         <v>89</v>
       </c>
@@ -2139,16 +2248,16 @@
         <v>3</v>
       </c>
       <c r="C91">
-        <v>425.99687499999987</v>
+        <v>425.9968749999999</v>
       </c>
       <c r="D91">
-        <v>66.365625000000009</v>
+        <v>66.36562500000001</v>
       </c>
       <c r="E91" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5">
       <c r="A92" s="1">
         <v>90</v>
       </c>
@@ -2156,16 +2265,16 @@
         <v>1</v>
       </c>
       <c r="C92">
-        <v>402.18124999999998</v>
+        <v>402.18125</v>
       </c>
       <c r="D92">
-        <v>53.425000000000011</v>
+        <v>53.42500000000001</v>
       </c>
       <c r="E92" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5">
       <c r="A93" s="1">
         <v>91</v>
       </c>
@@ -2173,16 +2282,16 @@
         <v>2</v>
       </c>
       <c r="C93">
-        <v>158.67500000000001</v>
+        <v>158.675</v>
       </c>
       <c r="D93">
-        <v>29.715624999999999</v>
+        <v>29.715625</v>
       </c>
       <c r="E93" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5">
       <c r="A94" s="1">
         <v>92</v>
       </c>
@@ -2190,16 +2299,16 @@
         <v>3</v>
       </c>
       <c r="C94">
-        <v>627.30312500000002</v>
+        <v>627.303125</v>
       </c>
       <c r="D94">
-        <v>76.371875000000017</v>
+        <v>76.37187500000002</v>
       </c>
       <c r="E94" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5">
       <c r="A95" s="1">
         <v>93</v>
       </c>
@@ -2207,16 +2316,16 @@
         <v>1</v>
       </c>
       <c r="C95">
-        <v>324.81249999999989</v>
+        <v>324.8124999999999</v>
       </c>
       <c r="D95">
         <v>48.71875</v>
       </c>
       <c r="E95" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5">
       <c r="A96" s="1">
         <v>94</v>
       </c>
@@ -2224,16 +2333,16 @@
         <v>2</v>
       </c>
       <c r="C96">
-        <v>136.69999999999999</v>
+        <v>136.7</v>
       </c>
       <c r="D96">
         <v>30.34375</v>
       </c>
       <c r="E96" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5">
       <c r="A97" s="1">
         <v>95</v>
       </c>
@@ -2241,16 +2350,16 @@
         <v>3</v>
       </c>
       <c r="C97">
-        <v>598.91250000000002</v>
+        <v>598.9125</v>
       </c>
       <c r="D97">
         <v>75.88124999999998</v>
       </c>
       <c r="E97" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5">
       <c r="A98" s="1">
         <v>96</v>
       </c>
@@ -2258,16 +2367,16 @@
         <v>1</v>
       </c>
       <c r="C98">
-        <v>425.78749999999991</v>
+        <v>425.7874999999999</v>
       </c>
       <c r="D98">
-        <v>57.834375000000001</v>
+        <v>57.834375</v>
       </c>
       <c r="E98" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5">
       <c r="A99" s="1">
         <v>97</v>
       </c>
@@ -2281,10 +2390,10 @@
         <v>29.1</v>
       </c>
       <c r="E99" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5">
       <c r="A100" s="1">
         <v>98</v>
       </c>
@@ -2292,16 +2401,16 @@
         <v>3</v>
       </c>
       <c r="C100">
-        <v>595.91874999999993</v>
+        <v>595.9187499999999</v>
       </c>
       <c r="D100">
-        <v>65.062500000000014</v>
+        <v>65.06250000000001</v>
       </c>
       <c r="E100" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5">
       <c r="A101" s="1">
         <v>99</v>
       </c>
@@ -2309,16 +2418,16 @@
         <v>1</v>
       </c>
       <c r="C101">
-        <v>494.77499999999998</v>
+        <v>494.775</v>
       </c>
       <c r="D101">
-        <v>65.493749999999977</v>
+        <v>65.49374999999998</v>
       </c>
       <c r="E101" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5">
       <c r="A102" s="1">
         <v>100</v>
       </c>
@@ -2326,16 +2435,16 @@
         <v>2</v>
       </c>
       <c r="C102">
-        <v>180.25625000000011</v>
+        <v>180.2562500000001</v>
       </c>
       <c r="D102">
-        <v>34.478124999999999</v>
+        <v>34.478125</v>
       </c>
       <c r="E102" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5">
       <c r="A103" s="1">
         <v>101</v>
       </c>
@@ -2343,16 +2452,16 @@
         <v>3</v>
       </c>
       <c r="C103">
-        <v>646.55000000000007</v>
+        <v>646.5500000000001</v>
       </c>
       <c r="D103">
-        <v>75.506249999999994</v>
+        <v>75.50624999999999</v>
       </c>
       <c r="E103" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5">
       <c r="A104" s="1">
         <v>102</v>
       </c>
@@ -2360,16 +2469,16 @@
         <v>1</v>
       </c>
       <c r="C104">
-        <v>467.77187500000002</v>
+        <v>467.771875</v>
       </c>
       <c r="D104">
-        <v>63.712500000000013</v>
+        <v>63.71250000000001</v>
       </c>
       <c r="E104" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5">
       <c r="A105" s="1">
         <v>103</v>
       </c>
@@ -2383,10 +2492,10 @@
         <v>23.95</v>
       </c>
       <c r="E105" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5">
       <c r="A106" s="1">
         <v>104</v>
       </c>
@@ -2394,16 +2503,16 @@
         <v>3</v>
       </c>
       <c r="C106">
-        <v>685.95624999999995</v>
+        <v>685.95625</v>
       </c>
       <c r="D106">
-        <v>84.100000000000009</v>
+        <v>84.10000000000001</v>
       </c>
       <c r="E106" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5">
       <c r="A107" s="1">
         <v>105</v>
       </c>
@@ -2411,16 +2520,16 @@
         <v>1</v>
       </c>
       <c r="C107">
-        <v>631.40312500000016</v>
+        <v>631.4031250000002</v>
       </c>
       <c r="D107">
-        <v>74.887500000000017</v>
+        <v>74.88750000000002</v>
       </c>
       <c r="E107" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5">
       <c r="A108" s="1">
         <v>106</v>
       </c>
@@ -2428,16 +2537,16 @@
         <v>2</v>
       </c>
       <c r="C108">
-        <v>83.543750000000031</v>
+        <v>83.54375000000003</v>
       </c>
       <c r="D108">
         <v>21.515625</v>
       </c>
       <c r="E108" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5">
       <c r="A109" s="1">
         <v>107</v>
       </c>
@@ -2445,16 +2554,16 @@
         <v>3</v>
       </c>
       <c r="C109">
-        <v>764.43124999999975</v>
+        <v>764.4312499999997</v>
       </c>
       <c r="D109">
-        <v>83.931249999999991</v>
+        <v>83.93124999999999</v>
       </c>
       <c r="E109" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5">
       <c r="A110" s="1">
         <v>108</v>
       </c>
@@ -2462,16 +2571,16 @@
         <v>1</v>
       </c>
       <c r="C110">
-        <v>759.33124999999995</v>
+        <v>759.33125</v>
       </c>
       <c r="D110">
-        <v>81.521875000000009</v>
+        <v>81.52187500000001</v>
       </c>
       <c r="E110" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5">
       <c r="A111" s="1">
         <v>109</v>
       </c>
@@ -2479,16 +2588,16 @@
         <v>2</v>
       </c>
       <c r="C111">
-        <v>165.74687499999999</v>
+        <v>165.746875</v>
       </c>
       <c r="D111">
-        <v>31.459375000000001</v>
+        <v>31.459375</v>
       </c>
       <c r="E111" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5">
       <c r="A112" s="1">
         <v>110</v>
       </c>
@@ -2496,16 +2605,16 @@
         <v>3</v>
       </c>
       <c r="C112">
-        <v>596.43125000000009</v>
+        <v>596.4312500000001</v>
       </c>
       <c r="D112">
-        <v>75.681250000000006</v>
+        <v>75.68125000000001</v>
       </c>
       <c r="E112" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5">
       <c r="A113" s="1">
         <v>111</v>
       </c>
@@ -2513,16 +2622,16 @@
         <v>1</v>
       </c>
       <c r="C113">
-        <v>863.14375000000018</v>
+        <v>863.1437500000002</v>
       </c>
       <c r="D113">
-        <v>94.681249999999991</v>
+        <v>94.68124999999999</v>
       </c>
       <c r="E113" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5">
       <c r="A114" s="1">
         <v>112</v>
       </c>
@@ -2530,16 +2639,16 @@
         <v>2</v>
       </c>
       <c r="C114">
-        <v>174.26875000000001</v>
+        <v>174.26875</v>
       </c>
       <c r="D114">
-        <v>31.831250000000001</v>
+        <v>31.83125</v>
       </c>
       <c r="E114" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5">
       <c r="A115" s="1">
         <v>113</v>
       </c>
@@ -2547,16 +2656,16 @@
         <v>3</v>
       </c>
       <c r="C115">
-        <v>792.84062500000005</v>
+        <v>792.840625</v>
       </c>
       <c r="D115">
-        <v>85.484374999999986</v>
+        <v>85.48437499999999</v>
       </c>
       <c r="E115" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5">
       <c r="A116" s="1">
         <v>114</v>
       </c>
@@ -2564,16 +2673,16 @@
         <v>1</v>
       </c>
       <c r="C116">
-        <v>748.00625000000002</v>
+        <v>748.00625</v>
       </c>
       <c r="D116">
-        <v>89.909374999999983</v>
+        <v>89.90937499999998</v>
       </c>
       <c r="E116" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5">
       <c r="A117" s="1">
         <v>115</v>
       </c>
@@ -2581,16 +2690,16 @@
         <v>2</v>
       </c>
       <c r="C117">
-        <v>145.52187499999999</v>
+        <v>145.521875</v>
       </c>
       <c r="D117">
-        <v>28.209374999999991</v>
+        <v>28.20937499999999</v>
       </c>
       <c r="E117" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5">
       <c r="A118" s="1">
         <v>116</v>
       </c>
@@ -2598,16 +2707,16 @@
         <v>3</v>
       </c>
       <c r="C118">
-        <v>888.72812499999998</v>
+        <v>888.728125</v>
       </c>
       <c r="D118">
-        <v>78.778125000000003</v>
+        <v>78.778125</v>
       </c>
       <c r="E118" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5">
       <c r="A119" s="1">
         <v>117</v>
       </c>
@@ -2615,16 +2724,16 @@
         <v>1</v>
       </c>
       <c r="C119">
-        <v>535.19687500000009</v>
+        <v>535.1968750000001</v>
       </c>
       <c r="D119">
         <v>81.53749999999998</v>
       </c>
       <c r="E119" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5">
       <c r="A120" s="1">
         <v>118</v>
       </c>
@@ -2632,16 +2741,16 @@
         <v>2</v>
       </c>
       <c r="C120">
-        <v>141.80937499999999</v>
+        <v>141.809375</v>
       </c>
       <c r="D120">
-        <v>28.934374999999999</v>
+        <v>28.934375</v>
       </c>
       <c r="E120" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5">
       <c r="A121" s="1">
         <v>119</v>
       </c>
@@ -2649,16 +2758,16 @@
         <v>3</v>
       </c>
       <c r="C121">
-        <v>883.80625000000009</v>
+        <v>883.8062500000001</v>
       </c>
       <c r="D121">
-        <v>79.990624999999994</v>
+        <v>79.99062499999999</v>
       </c>
       <c r="E121" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5">
       <c r="A122" s="1">
         <v>120</v>
       </c>
@@ -2666,16 +2775,16 @@
         <v>1</v>
       </c>
       <c r="C122">
-        <v>543.66250000000002</v>
+        <v>543.6625</v>
       </c>
       <c r="D122">
         <v>87.28125</v>
       </c>
       <c r="E122" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5">
       <c r="A123" s="1">
         <v>121</v>
       </c>
@@ -2686,13 +2795,13 @@
         <v>124.91875</v>
       </c>
       <c r="D123">
-        <v>27.871874999999999</v>
+        <v>27.871875</v>
       </c>
       <c r="E123" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5">
       <c r="A124" s="1">
         <v>122</v>
       </c>
@@ -2700,16 +2809,16 @@
         <v>3</v>
       </c>
       <c r="C124">
-        <v>796.98124999999982</v>
+        <v>796.9812499999998</v>
       </c>
       <c r="D124">
-        <v>75.615625000000009</v>
+        <v>75.61562500000001</v>
       </c>
       <c r="E124" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5">
       <c r="A125" s="1">
         <v>123</v>
       </c>
@@ -2717,16 +2826,16 @@
         <v>1</v>
       </c>
       <c r="C125">
-        <v>738.00624999999991</v>
+        <v>738.0062499999999</v>
       </c>
       <c r="D125">
-        <v>88.162500000000009</v>
+        <v>88.16250000000001</v>
       </c>
       <c r="E125" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5">
       <c r="A126" s="1">
         <v>124</v>
       </c>
@@ -2734,16 +2843,16 @@
         <v>2</v>
       </c>
       <c r="C126">
-        <v>104.38124999999999</v>
+        <v>104.38125</v>
       </c>
       <c r="D126">
-        <v>26.368749999999999</v>
+        <v>26.36875</v>
       </c>
       <c r="E126" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5">
       <c r="A127" s="1">
         <v>125</v>
       </c>
@@ -2751,16 +2860,16 @@
         <v>3</v>
       </c>
       <c r="C127">
-        <v>926.86249999999995</v>
+        <v>926.8625</v>
       </c>
       <c r="D127">
-        <v>87.612500000000011</v>
+        <v>87.61250000000001</v>
       </c>
       <c r="E127" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5">
       <c r="A128" s="1">
         <v>126</v>
       </c>
@@ -2768,16 +2877,16 @@
         <v>1</v>
       </c>
       <c r="C128">
-        <v>864.20000000000027</v>
+        <v>864.2000000000003</v>
       </c>
       <c r="D128">
-        <v>93.731250000000003</v>
+        <v>93.73125</v>
       </c>
       <c r="E128" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5">
       <c r="A129" s="1">
         <v>127</v>
       </c>
@@ -2785,16 +2894,16 @@
         <v>2</v>
       </c>
       <c r="C129">
-        <v>137.61250000000001</v>
+        <v>137.6125</v>
       </c>
       <c r="D129">
-        <v>29.831250000000001</v>
+        <v>29.83125</v>
       </c>
       <c r="E129" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5">
       <c r="A130" s="1">
         <v>128</v>
       </c>
@@ -2802,16 +2911,16 @@
         <v>3</v>
       </c>
       <c r="C130">
-        <v>852.03437500000007</v>
+        <v>852.0343750000001</v>
       </c>
       <c r="D130">
-        <v>90.771875000000009</v>
+        <v>90.77187500000001</v>
       </c>
       <c r="E130" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5">
       <c r="A131" s="1">
         <v>129</v>
       </c>
@@ -2819,16 +2928,16 @@
         <v>1</v>
       </c>
       <c r="C131">
-        <v>749.31562500000007</v>
+        <v>749.3156250000001</v>
       </c>
       <c r="D131">
         <v>90.140625</v>
       </c>
       <c r="E131" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5">
       <c r="A132" s="1">
         <v>130</v>
       </c>
@@ -2836,16 +2945,16 @@
         <v>2</v>
       </c>
       <c r="C132">
-        <v>98.184374999999974</v>
+        <v>98.18437499999997</v>
       </c>
       <c r="D132">
-        <v>26.440625000000001</v>
+        <v>26.440625</v>
       </c>
       <c r="E132" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5">
       <c r="A133" s="1">
         <v>131</v>
       </c>
@@ -2853,16 +2962,16 @@
         <v>3</v>
       </c>
       <c r="C133">
-        <v>887.07812499999989</v>
+        <v>887.0781249999999</v>
       </c>
       <c r="D133">
-        <v>94.615625000000009</v>
+        <v>94.61562500000001</v>
       </c>
       <c r="E133" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5">
       <c r="A134" s="1">
         <v>132</v>
       </c>
@@ -2870,16 +2979,16 @@
         <v>1</v>
       </c>
       <c r="C134">
-        <v>595.17500000000018</v>
+        <v>595.1750000000002</v>
       </c>
       <c r="D134">
-        <v>86.918750000000031</v>
+        <v>86.91875000000003</v>
       </c>
       <c r="E134" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5">
       <c r="A135" s="1">
         <v>133</v>
       </c>
@@ -2887,16 +2996,16 @@
         <v>2</v>
       </c>
       <c r="C135">
-        <v>98.040625000000006</v>
+        <v>98.04062500000001</v>
       </c>
       <c r="D135">
-        <v>23.818750000000001</v>
+        <v>23.81875</v>
       </c>
       <c r="E135" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5">
       <c r="A136" s="1">
         <v>134</v>
       </c>
@@ -2904,16 +3013,16 @@
         <v>3</v>
       </c>
       <c r="C136">
-        <v>841.91562499999998</v>
+        <v>841.915625</v>
       </c>
       <c r="D136">
-        <v>94.434375000000003</v>
+        <v>94.434375</v>
       </c>
       <c r="E136" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5">
       <c r="A137" s="1">
         <v>135</v>
       </c>
@@ -2921,16 +3030,16 @@
         <v>1</v>
       </c>
       <c r="C137">
-        <v>629.48125000000016</v>
+        <v>629.4812500000002</v>
       </c>
       <c r="D137">
-        <v>87.806250000000006</v>
+        <v>87.80625000000001</v>
       </c>
       <c r="E137" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5">
       <c r="A138" s="1">
         <v>136</v>
       </c>
@@ -2938,16 +3047,16 @@
         <v>2</v>
       </c>
       <c r="C138">
-        <v>110.92812499999999</v>
+        <v>110.928125</v>
       </c>
       <c r="D138">
-        <v>25.915625000000009</v>
+        <v>25.91562500000001</v>
       </c>
       <c r="E138" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5">
       <c r="A139" s="1">
         <v>137</v>
       </c>
@@ -2955,16 +3064,16 @@
         <v>3</v>
       </c>
       <c r="C139">
-        <v>945.89687499999991</v>
+        <v>945.8968749999999</v>
       </c>
       <c r="D139">
         <v>108.8625</v>
       </c>
       <c r="E139" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5">
       <c r="A140" s="1">
         <v>138</v>
       </c>
@@ -2972,16 +3081,16 @@
         <v>1</v>
       </c>
       <c r="C140">
-        <v>860.03750000000002</v>
+        <v>860.0375</v>
       </c>
       <c r="D140">
-        <v>94.674999999999983</v>
+        <v>94.67499999999998</v>
       </c>
       <c r="E140" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5">
       <c r="A141" s="1">
         <v>139</v>
       </c>
@@ -2989,16 +3098,16 @@
         <v>2</v>
       </c>
       <c r="C141">
-        <v>128.86875000000001</v>
+        <v>128.86875</v>
       </c>
       <c r="D141">
-        <v>30.406249999999989</v>
+        <v>30.40624999999999</v>
       </c>
       <c r="E141" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5">
       <c r="A142" s="1">
         <v>140</v>
       </c>
@@ -3006,16 +3115,16 @@
         <v>3</v>
       </c>
       <c r="C142">
-        <v>779.11250000000007</v>
+        <v>779.1125000000001</v>
       </c>
       <c r="D142">
-        <v>100.97499999999999</v>
+        <v>100.975</v>
       </c>
       <c r="E142" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5">
       <c r="A143" s="1">
         <v>141</v>
       </c>
@@ -3029,10 +3138,10 @@
         <v>100.034375</v>
       </c>
       <c r="E143" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5">
       <c r="A144" s="1">
         <v>142</v>
       </c>
@@ -3043,13 +3152,13 @@
         <v>191.0187499999999</v>
       </c>
       <c r="D144">
-        <v>31.165624999999999</v>
+        <v>31.165625</v>
       </c>
       <c r="E144" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5">
       <c r="A145" s="1">
         <v>143</v>
       </c>
@@ -3057,16 +3166,16 @@
         <v>3</v>
       </c>
       <c r="C145">
-        <v>730.47187499999995</v>
+        <v>730.471875</v>
       </c>
       <c r="D145">
-        <v>93.040625000000006</v>
+        <v>93.04062500000001</v>
       </c>
       <c r="E145" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5">
       <c r="A146" s="1">
         <v>144</v>
       </c>
@@ -3074,16 +3183,16 @@
         <v>1</v>
       </c>
       <c r="C146">
-        <v>1187.6468749999999</v>
+        <v>1187.646875</v>
       </c>
       <c r="D146">
         <v>112.878125</v>
       </c>
       <c r="E146" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5">
       <c r="A147" s="1">
         <v>145</v>
       </c>
@@ -3091,16 +3200,16 @@
         <v>2</v>
       </c>
       <c r="C147">
-        <v>145.61562499999999</v>
+        <v>145.615625</v>
       </c>
       <c r="D147">
-        <v>27.481249999999999</v>
+        <v>27.48125</v>
       </c>
       <c r="E147" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5">
       <c r="A148" s="1">
         <v>146</v>
       </c>
@@ -3108,16 +3217,16 @@
         <v>3</v>
       </c>
       <c r="C148">
-        <v>768.93437500000016</v>
+        <v>768.9343750000002</v>
       </c>
       <c r="D148">
         <v>101.8875</v>
       </c>
       <c r="E148" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5">
       <c r="A149" s="1">
         <v>147</v>
       </c>
@@ -3131,10 +3240,10 @@
         <v>119.55</v>
       </c>
       <c r="E149" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5">
       <c r="A150" s="1">
         <v>148</v>
       </c>
@@ -3142,16 +3251,16 @@
         <v>2</v>
       </c>
       <c r="C150">
-        <v>135.66249999999999</v>
+        <v>135.6625</v>
       </c>
       <c r="D150">
-        <v>32.209374999999987</v>
+        <v>32.20937499999999</v>
       </c>
       <c r="E150" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5">
       <c r="A151" s="1">
         <v>149</v>
       </c>
@@ -3165,10 +3274,10 @@
         <v>113.046875</v>
       </c>
       <c r="E151" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5">
       <c r="A152" s="1">
         <v>150</v>
       </c>
@@ -3179,13 +3288,13 @@
         <v>1486.4375</v>
       </c>
       <c r="D152">
-        <v>135.79374999999999</v>
+        <v>135.79375</v>
       </c>
       <c r="E152" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5">
       <c r="A153" s="1">
         <v>151</v>
       </c>
@@ -3196,13 +3305,13 @@
         <v>155.171875</v>
       </c>
       <c r="D153">
-        <v>33.037499999999987</v>
+        <v>33.03749999999999</v>
       </c>
       <c r="E153" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5">
       <c r="A154" s="1">
         <v>152</v>
       </c>
@@ -3210,16 +3319,16 @@
         <v>3</v>
       </c>
       <c r="C154">
-        <v>963.25312500000007</v>
+        <v>963.2531250000001</v>
       </c>
       <c r="D154">
-        <v>107.71250000000001</v>
+        <v>107.7125</v>
       </c>
       <c r="E154" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5">
       <c r="A155" s="1">
         <v>153</v>
       </c>
@@ -3230,13 +3339,13 @@
         <v>1097.9375</v>
       </c>
       <c r="D155">
-        <v>110.49062499999999</v>
+        <v>110.490625</v>
       </c>
       <c r="E155" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5">
       <c r="A156" s="1">
         <v>154</v>
       </c>
@@ -3247,13 +3356,13 @@
         <v>117.21875</v>
       </c>
       <c r="D156">
-        <v>32.725000000000001</v>
+        <v>32.725</v>
       </c>
       <c r="E156" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5">
       <c r="A157" s="1">
         <v>155</v>
       </c>
@@ -3267,10 +3376,10 @@
         <v>114.175</v>
       </c>
       <c r="E157" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5">
       <c r="A158" s="1">
         <v>156</v>
       </c>
@@ -3284,10 +3393,10 @@
         <v>103.309375</v>
       </c>
       <c r="E158" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5">
       <c r="A159" s="1">
         <v>157</v>
       </c>
@@ -3295,16 +3404,16 @@
         <v>2</v>
       </c>
       <c r="C159">
-        <v>128.31874999999999</v>
+        <v>128.31875</v>
       </c>
       <c r="D159">
-        <v>31.634374999999991</v>
+        <v>31.63437499999999</v>
       </c>
       <c r="E159" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5">
       <c r="A160" s="1">
         <v>158</v>
       </c>
@@ -3312,16 +3421,16 @@
         <v>3</v>
       </c>
       <c r="C160">
-        <v>1236.7281250000001</v>
+        <v>1236.728125</v>
       </c>
       <c r="D160">
         <v>122.35625</v>
       </c>
       <c r="E160" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5">
       <c r="A161" s="1">
         <v>159</v>
       </c>
@@ -3332,13 +3441,13 @@
         <v>1232.54375</v>
       </c>
       <c r="D161">
-        <v>114.21250000000001</v>
+        <v>114.2125</v>
       </c>
       <c r="E161" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5">
       <c r="A162" s="1">
         <v>160</v>
       </c>
@@ -3352,10 +3461,10 @@
         <v>29.296875</v>
       </c>
       <c r="E162" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5">
       <c r="A163" s="1">
         <v>161</v>
       </c>
@@ -3363,16 +3472,16 @@
         <v>3</v>
       </c>
       <c r="C163">
-        <v>914.87812499999984</v>
+        <v>914.8781249999998</v>
       </c>
       <c r="D163">
         <v>106.65625</v>
       </c>
       <c r="E163" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5">
       <c r="A164" s="1">
         <v>162</v>
       </c>
@@ -3380,16 +3489,16 @@
         <v>1</v>
       </c>
       <c r="C164">
-        <v>1479.6031250000001</v>
+        <v>1479.603125</v>
       </c>
       <c r="D164">
-        <v>128.92500000000001</v>
+        <v>128.925</v>
       </c>
       <c r="E164" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5">
       <c r="A165" s="1">
         <v>163</v>
       </c>
@@ -3397,16 +3506,16 @@
         <v>2</v>
       </c>
       <c r="C165">
-        <v>101.75937500000001</v>
+        <v>101.759375</v>
       </c>
       <c r="D165">
         <v>28.03125</v>
       </c>
       <c r="E165" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5">
       <c r="A166" s="1">
         <v>164</v>
       </c>
@@ -3417,13 +3526,13 @@
         <v>1401.6125</v>
       </c>
       <c r="D166">
-        <v>124.04062500000001</v>
+        <v>124.040625</v>
       </c>
       <c r="E166" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5">
       <c r="A167" s="1">
         <v>165</v>
       </c>
@@ -3434,13 +3543,13 @@
         <v>1623.903125</v>
       </c>
       <c r="D167">
-        <v>140.93437499999999</v>
+        <v>140.934375</v>
       </c>
       <c r="E167" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5">
       <c r="A168" s="1">
         <v>166</v>
       </c>
@@ -3454,10 +3563,10 @@
         <v>26.640625</v>
       </c>
       <c r="E168" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5">
       <c r="A169" s="1">
         <v>167</v>
       </c>
@@ -3468,13 +3577,13 @@
         <v>1536.128125</v>
       </c>
       <c r="D169">
-        <v>137.72499999999999</v>
+        <v>137.725</v>
       </c>
       <c r="E169" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5">
       <c r="A170" s="1">
         <v>168</v>
       </c>
@@ -3485,13 +3594,13 @@
         <v>1939.596875</v>
       </c>
       <c r="D170">
-        <v>151.35312500000001</v>
+        <v>151.353125</v>
       </c>
       <c r="E170" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5">
       <c r="A171" s="1">
         <v>169</v>
       </c>
@@ -3499,16 +3608,16 @@
         <v>2</v>
       </c>
       <c r="C171">
-        <v>90.018749999999997</v>
+        <v>90.01875</v>
       </c>
       <c r="D171">
-        <v>27.840624999999999</v>
+        <v>27.840625</v>
       </c>
       <c r="E171" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5">
       <c r="A172" s="1">
         <v>170</v>
       </c>
@@ -3516,16 +3625,16 @@
         <v>3</v>
       </c>
       <c r="C172">
-        <v>1168.0093750000001</v>
+        <v>1168.009375</v>
       </c>
       <c r="D172">
         <v>127.003125</v>
       </c>
       <c r="E172" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5">
       <c r="A173" s="1">
         <v>171</v>
       </c>
@@ -3536,13 +3645,13 @@
         <v>2005.071874999999</v>
       </c>
       <c r="D173">
-        <v>159.23750000000001</v>
+        <v>159.2375</v>
       </c>
       <c r="E173" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5">
       <c r="A174" s="1">
         <v>172</v>
       </c>
@@ -3550,16 +3659,16 @@
         <v>2</v>
       </c>
       <c r="C174">
-        <v>153.23437499999989</v>
+        <v>153.2343749999999</v>
       </c>
       <c r="D174">
         <v>34.33124999999999</v>
       </c>
       <c r="E174" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5">
       <c r="A175" s="1">
         <v>173</v>
       </c>
@@ -3573,10 +3682,10 @@
         <v>126.875</v>
       </c>
       <c r="E175" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5">
       <c r="A176" s="1">
         <v>174</v>
       </c>
@@ -3584,16 +3693,16 @@
         <v>1</v>
       </c>
       <c r="C176">
-        <v>1873.8843750000001</v>
+        <v>1873.884375</v>
       </c>
       <c r="D176">
-        <v>144.67500000000001</v>
+        <v>144.675</v>
       </c>
       <c r="E176" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5">
       <c r="A177" s="1">
         <v>175</v>
       </c>
@@ -3601,16 +3710,16 @@
         <v>2</v>
       </c>
       <c r="C177">
-        <v>117.22499999999999</v>
+        <v>117.225</v>
       </c>
       <c r="D177">
         <v>24.515625</v>
       </c>
       <c r="E177" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5">
       <c r="A178" s="1">
         <v>176</v>
       </c>
@@ -3621,13 +3730,13 @@
         <v>1169.51875</v>
       </c>
       <c r="D178">
-        <v>133.02812499999999</v>
+        <v>133.028125</v>
       </c>
       <c r="E178" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5">
       <c r="A179" s="1">
         <v>177</v>
       </c>
@@ -3638,13 +3747,13 @@
         <v>1695.421875</v>
       </c>
       <c r="D179">
-        <v>157.05000000000001</v>
+        <v>157.05</v>
       </c>
       <c r="E179" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5">
       <c r="A180" s="1">
         <v>178</v>
       </c>
@@ -3652,16 +3761,16 @@
         <v>2</v>
       </c>
       <c r="C180">
-        <v>106.77187499999999</v>
+        <v>106.771875</v>
       </c>
       <c r="D180">
-        <v>27.415624999999999</v>
+        <v>27.415625</v>
       </c>
       <c r="E180" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5">
       <c r="A181" s="1">
         <v>179</v>
       </c>
@@ -3672,13 +3781,13 @@
         <v>1400.23125</v>
       </c>
       <c r="D181">
-        <v>155.12187499999999</v>
+        <v>155.121875</v>
       </c>
       <c r="E181" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5">
       <c r="A182" s="1">
         <v>180</v>
       </c>
@@ -3686,16 +3795,16 @@
         <v>1</v>
       </c>
       <c r="C182">
-        <v>1632.0374999999999</v>
+        <v>1632.0375</v>
       </c>
       <c r="D182">
-        <v>144.60312500000001</v>
+        <v>144.603125</v>
       </c>
       <c r="E182" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5">
       <c r="A183" s="1">
         <v>181</v>
       </c>
@@ -3709,10 +3818,10 @@
         <v>26.46875</v>
       </c>
       <c r="E183" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5">
       <c r="A184" s="1">
         <v>182</v>
       </c>
@@ -3720,16 +3829,16 @@
         <v>3</v>
       </c>
       <c r="C184">
-        <v>1310.5562500000001</v>
+        <v>1310.55625</v>
       </c>
       <c r="D184">
-        <v>161.55000000000001</v>
+        <v>161.55</v>
       </c>
       <c r="E184" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5">
       <c r="A185" s="1">
         <v>183</v>
       </c>
@@ -3737,16 +3846,16 @@
         <v>1</v>
       </c>
       <c r="C185">
-        <v>2074.2218750000002</v>
+        <v>2074.221875</v>
       </c>
       <c r="D185">
-        <v>159.64687499999999</v>
+        <v>159.646875</v>
       </c>
       <c r="E185" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5">
       <c r="A186" s="1">
         <v>184</v>
       </c>
@@ -3754,16 +3863,16 @@
         <v>2</v>
       </c>
       <c r="C186">
-        <v>219.91562500000001</v>
+        <v>219.915625</v>
       </c>
       <c r="D186">
         <v>39.375</v>
       </c>
       <c r="E186" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5">
       <c r="A187" s="1">
         <v>185</v>
       </c>
@@ -3771,16 +3880,16 @@
         <v>3</v>
       </c>
       <c r="C187">
-        <v>1236.5250000000001</v>
+        <v>1236.525</v>
       </c>
       <c r="D187">
-        <v>154.27500000000001</v>
+        <v>154.275</v>
       </c>
       <c r="E187" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="188" spans="1:5">
       <c r="A188" s="1">
         <v>186</v>
       </c>
@@ -3788,16 +3897,16 @@
         <v>1</v>
       </c>
       <c r="C188">
-        <v>2077.3156250000011</v>
+        <v>2077.315625000001</v>
       </c>
       <c r="D188">
         <v>168.78125</v>
       </c>
       <c r="E188" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5">
       <c r="A189" s="1">
         <v>187</v>
       </c>
@@ -3805,16 +3914,16 @@
         <v>2</v>
       </c>
       <c r="C189">
-        <v>203.30625000000001</v>
+        <v>203.30625</v>
       </c>
       <c r="D189">
-        <v>39.193750000000001</v>
+        <v>39.19375</v>
       </c>
       <c r="E189" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5">
       <c r="A190" s="1">
         <v>188</v>
       </c>
@@ -3822,16 +3931,16 @@
         <v>3</v>
       </c>
       <c r="C190">
-        <v>1111.9906249999999</v>
+        <v>1111.990625</v>
       </c>
       <c r="D190">
-        <v>145.75624999999999</v>
+        <v>145.75625</v>
       </c>
       <c r="E190" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5">
       <c r="A191" s="1">
         <v>189</v>
       </c>
@@ -3842,13 +3951,13 @@
         <v>1955.15625</v>
       </c>
       <c r="D191">
-        <v>147.02500000000001</v>
+        <v>147.025</v>
       </c>
       <c r="E191" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5">
       <c r="A192" s="1">
         <v>190</v>
       </c>
@@ -3856,16 +3965,16 @@
         <v>2</v>
       </c>
       <c r="C192">
-        <v>188.66562500000001</v>
+        <v>188.665625</v>
       </c>
       <c r="D192">
-        <v>42.731250000000003</v>
+        <v>42.73125</v>
       </c>
       <c r="E192" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5">
       <c r="A193" s="1">
         <v>191</v>
       </c>
@@ -3873,16 +3982,16 @@
         <v>3</v>
       </c>
       <c r="C193">
-        <v>934.53437499999995</v>
+        <v>934.534375</v>
       </c>
       <c r="D193">
-        <v>135.77187499999999</v>
+        <v>135.771875</v>
       </c>
       <c r="E193" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5">
       <c r="A194" s="1">
         <v>192</v>
       </c>
@@ -3893,13 +4002,13 @@
         <v>2038.1875</v>
       </c>
       <c r="D194">
-        <v>149.31874999999999</v>
+        <v>149.31875</v>
       </c>
       <c r="E194" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5">
       <c r="A195" s="1">
         <v>193</v>
       </c>
@@ -3910,13 +4019,13 @@
         <v>155.7156249999999</v>
       </c>
       <c r="D195">
-        <v>37.221874999999997</v>
+        <v>37.221875</v>
       </c>
       <c r="E195" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5">
       <c r="A196" s="1">
         <v>194</v>
       </c>
@@ -3924,16 +4033,16 @@
         <v>3</v>
       </c>
       <c r="C196">
-        <v>888.17500000000018</v>
+        <v>888.1750000000002</v>
       </c>
       <c r="D196">
         <v>126.421875</v>
       </c>
       <c r="E196" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5">
       <c r="A197" s="1">
         <v>195</v>
       </c>
@@ -3944,13 +4053,13 @@
         <v>1837.153125000001</v>
       </c>
       <c r="D197">
-        <v>132.17812499999999</v>
+        <v>132.178125</v>
       </c>
       <c r="E197" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5">
       <c r="A198" s="1">
         <v>196</v>
       </c>
@@ -3961,13 +4070,13 @@
         <v>160.4375</v>
       </c>
       <c r="D198">
-        <v>35.393749999999997</v>
+        <v>35.39375</v>
       </c>
       <c r="E198" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5">
       <c r="A199" s="1">
         <v>197</v>
       </c>
@@ -3975,13 +4084,13 @@
         <v>3</v>
       </c>
       <c r="C199">
-        <v>894.75625000000002</v>
+        <v>894.75625</v>
       </c>
       <c r="D199">
         <v>123.35625</v>
       </c>
       <c r="E199" t="s">
-        <v>69</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>